<commit_message>
Updated anmd run the whole architecture to calculate Specific Fuel Consumption on a different set of parameters. Also explained the results, and saved the confidence scores and models in the directories
</commit_message>
<xml_diff>
--- a/Results/SFC_Cruise_kg_s_N Inital_Predictions/Esemble_Confidence_Scores.xlsx
+++ b/Results/SFC_Cruise_kg_s_N Inital_Predictions/Esemble_Confidence_Scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,87 +457,87 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B2" t="n">
         <v>0.17142</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1713926185654125</v>
+        <v>0.171428956652766</v>
       </c>
       <c r="D2" t="n">
-        <v>2.738143458752562e-05</v>
+        <v>8.956652765984563e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9999726193151349</v>
+        <v>0.999991043427455</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" t="n">
         <v>0.15877</v>
       </c>
       <c r="C3" t="n">
-        <v>0.158736972759103</v>
+        <v>0.1588348147326499</v>
       </c>
       <c r="D3" t="n">
-        <v>3.302724089701559e-05</v>
+        <v>6.481473264993709e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9999669738498655</v>
+        <v>0.9999351894680274</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B4" t="n">
-        <v>0.17732</v>
+        <v>0.22481</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1776682842531389</v>
+        <v>0.2231413111608817</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0003482842531388752</v>
+        <v>0.001668688839118332</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9996518370065494</v>
+        <v>0.9983340910445625</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.17732</v>
+        <v>0.16776</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1769641196412943</v>
+        <v>0.1659385432086418</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0003558803587057346</v>
+        <v>0.0018214567913582</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9996442462470674</v>
+        <v>0.9981818548814158</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B6" t="n">
-        <v>0.17704</v>
+        <v>0.16776</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1766698268662702</v>
+        <v>0.1659385432086418</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0003701731337297787</v>
+        <v>0.0018214567913582</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9996299638437138</v>
+        <v>0.9981818548814158</v>
       </c>
     </row>
     <row r="7">
@@ -545,254 +545,254 @@
         <v>29</v>
       </c>
       <c r="B7" t="n">
-        <v>0.17704</v>
+        <v>0.15737</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1776997860070104</v>
+        <v>0.1594464066356196</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0006597860070104433</v>
+        <v>0.002076406635619615</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9993406490235377</v>
+        <v>0.9979278958950936</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>0.18153</v>
+        <v>0.16439</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1824411751138283</v>
+        <v>0.1664767301669309</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0009111751138283497</v>
+        <v>0.002086730166930922</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9990896543704542</v>
+        <v>0.9979176152082332</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B9" t="n">
-        <v>0.22481</v>
+        <v>0.22368</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2234390224830053</v>
+        <v>0.2213441903847347</v>
       </c>
       <c r="D9" t="n">
-        <v>0.001370977516994665</v>
+        <v>0.002335809615265305</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9986308994890245</v>
+        <v>0.9976696336767996</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B10" t="n">
-        <v>0.22481</v>
+        <v>0.15315</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2231925603079822</v>
+        <v>0.156088591248787</v>
       </c>
       <c r="D10" t="n">
-        <v>0.001617439692017858</v>
+        <v>0.002938591248786954</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9983851721945703</v>
+        <v>0.9970700187684193</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>0.21638</v>
+        <v>0.15315</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2181708462163904</v>
+        <v>0.156088591248787</v>
       </c>
       <c r="D11" t="n">
-        <v>0.001790846216390446</v>
+        <v>0.002938591248786954</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9982123551805706</v>
+        <v>0.9970700187684193</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" t="n">
-        <v>0.17423</v>
+        <v>0.15315</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1761531494658564</v>
+        <v>0.156088591248787</v>
       </c>
       <c r="D12" t="n">
-        <v>0.001923149465856394</v>
+        <v>0.002938591248786954</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9980805419388885</v>
+        <v>0.9970700187684193</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B13" t="n">
-        <v>0.16861</v>
+        <v>0.15315</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1712209502876217</v>
+        <v>0.156088591248787</v>
       </c>
       <c r="D13" t="n">
-        <v>0.002610950287621677</v>
+        <v>0.002938591248786954</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9973958490211255</v>
+        <v>0.9970700187684193</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B14" t="n">
-        <v>0.17788</v>
+        <v>0.16748</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1752396306014153</v>
+        <v>0.1642570642932437</v>
       </c>
       <c r="D14" t="n">
-        <v>0.002640369398584697</v>
+        <v>0.00322293570675633</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9973665837929822</v>
+        <v>0.9967874182377162</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B15" t="n">
-        <v>0.20233</v>
+        <v>0.16186</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1996328055692943</v>
+        <v>0.1651145987488062</v>
       </c>
       <c r="D15" t="n">
-        <v>0.002697194430705735</v>
+        <v>0.003254598748806181</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9973100608581665</v>
+        <v>0.9967559593019907</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" t="n">
-        <v>0.20458</v>
+        <v>0.17732</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2075120768891602</v>
+        <v>0.1738521128339571</v>
       </c>
       <c r="D16" t="n">
-        <v>0.002932076889160168</v>
+        <v>0.003467887166042932</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9970764950521329</v>
+        <v>0.9965440975138359</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B17" t="n">
-        <v>0.20233</v>
+        <v>0.1939</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1988888574191632</v>
+        <v>0.1974294051802059</v>
       </c>
       <c r="D17" t="n">
-        <v>0.003441142580836803</v>
+        <v>0.003529405180205891</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9965706582730043</v>
+        <v>0.9964830077105991</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" t="n">
-        <v>0.16748</v>
+        <v>0.18462</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1640035698345104</v>
+        <v>0.1810281619637109</v>
       </c>
       <c r="D18" t="n">
-        <v>0.003476430165489569</v>
+        <v>0.003591838036289097</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9965356135321323</v>
+        <v>0.9964210170906559</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
-        <v>0.16186</v>
+        <v>0.18266</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1654417257396719</v>
+        <v>0.178891989034667</v>
       </c>
       <c r="D19" t="n">
-        <v>0.003581725739671915</v>
+        <v>0.003768010965333024</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9964310572344947</v>
+        <v>0.9962461336442577</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>0.17648</v>
+        <v>0.16018</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1720593271183147</v>
+        <v>0.1641109707039884</v>
       </c>
       <c r="D20" t="n">
-        <v>0.004420672881685267</v>
+        <v>0.003930970703988401</v>
       </c>
       <c r="E20" t="n">
-        <v>0.995598783456933</v>
+        <v>0.9960844213210877</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B21" t="n">
-        <v>0.16355</v>
+        <v>0.16861</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1679788569795228</v>
+        <v>0.1726037236736787</v>
       </c>
       <c r="D21" t="n">
-        <v>0.004428856979522833</v>
+        <v>0.003993723673678701</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9955906713066358</v>
+        <v>0.9960221627092793</v>
       </c>
     </row>
     <row r="22">
@@ -800,152 +800,152 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>0.21666</v>
+        <v>0.18378</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2119079502281771</v>
+        <v>0.179775799818457</v>
       </c>
       <c r="D22" t="n">
-        <v>0.004752049771822864</v>
+        <v>0.004004200181542988</v>
       </c>
       <c r="E22" t="n">
-        <v>0.995270425402066</v>
+        <v>0.9960117694917821</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.16018</v>
+        <v>0.16861</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1655165820098765</v>
+        <v>0.1727121012152924</v>
       </c>
       <c r="D23" t="n">
-        <v>0.005336582009876523</v>
+        <v>0.00410210121529242</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9946917459233329</v>
+        <v>0.9959146572740685</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.19952</v>
+        <v>0.17732</v>
       </c>
       <c r="C24" t="n">
-        <v>0.205065168251342</v>
+        <v>0.173158783592591</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00554516825134202</v>
+        <v>0.004161216407409046</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9944854110721001</v>
+        <v>0.9958560275587056</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B25" t="n">
-        <v>0.18153</v>
+        <v>0.20711</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1756046440052423</v>
+        <v>0.2113230416875116</v>
       </c>
       <c r="D25" t="n">
-        <v>0.005925355994757658</v>
+        <v>0.004213041687511632</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9941095470360243</v>
+        <v>0.9958046335661684</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B26" t="n">
-        <v>0.18968</v>
+        <v>0.16158</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1961388050493744</v>
+        <v>0.1660880669640323</v>
       </c>
       <c r="D26" t="n">
-        <v>0.006458805049374378</v>
+        <v>0.004508066964032331</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9935826434057999</v>
+        <v>0.9955121644989301</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" t="n">
-        <v>0.16299</v>
+        <v>0.16158</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1696147957767241</v>
+        <v>0.1661076915302122</v>
       </c>
       <c r="D27" t="n">
-        <v>0.006624795776724118</v>
+        <v>0.004527691530212236</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9934188033073313</v>
+        <v>0.9954927160611022</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B28" t="n">
-        <v>0.22762</v>
+        <v>0.17535</v>
       </c>
       <c r="C28" t="n">
-        <v>0.2207481874558742</v>
+        <v>0.1707552234816436</v>
       </c>
       <c r="D28" t="n">
-        <v>0.006871812544125833</v>
+        <v>0.00459477651835638</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9931750869787859</v>
+        <v>0.9954262388917843</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B29" t="n">
-        <v>0.17423</v>
+        <v>0.17535</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1668789794556794</v>
+        <v>0.1706713675790318</v>
       </c>
       <c r="D29" t="n">
-        <v>0.007351020544320575</v>
+        <v>0.004678632420968221</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9927026226266704</v>
+        <v>0.9953431552438872</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1613</v>
+        <v>0.22762</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1688997082083079</v>
+        <v>0.2227701717392069</v>
       </c>
       <c r="D30" t="n">
-        <v>0.007599708208307909</v>
+        <v>0.004849828260793138</v>
       </c>
       <c r="E30" t="n">
-        <v>0.9924576117416494</v>
+        <v>0.9951735790519193</v>
       </c>
     </row>
     <row r="31">
@@ -953,322 +953,356 @@
         <v>43</v>
       </c>
       <c r="B31" t="n">
-        <v>0.17423</v>
+        <v>0.20682</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1666061203232456</v>
+        <v>0.2116749473021086</v>
       </c>
       <c r="D31" t="n">
-        <v>0.007623879676754375</v>
+        <v>0.004854947302108586</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9924338040904708</v>
+        <v>0.9951685093304825</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B32" t="n">
-        <v>0.18378</v>
+        <v>0.15315</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1748898897357302</v>
+        <v>0.1582000249363662</v>
       </c>
       <c r="D32" t="n">
-        <v>0.008890110264269835</v>
+        <v>0.005050024936366221</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9911882273660695</v>
+        <v>0.9949753496730812</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B33" t="n">
-        <v>0.18378</v>
+        <v>0.17704</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1747584720488964</v>
+        <v>0.1715426682470617</v>
       </c>
       <c r="D33" t="n">
-        <v>0.009021527951103558</v>
+        <v>0.005497331752938261</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9910591323364306</v>
+        <v>0.9945327236787844</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B34" t="n">
-        <v>0.17535</v>
+        <v>0.17985</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1849291339477093</v>
+        <v>0.1856202330115029</v>
       </c>
       <c r="D34" t="n">
-        <v>0.009579133947709262</v>
+        <v>0.005770233011502895</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9905117552199673</v>
+        <v>0.9942628715564334</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="B35" t="n">
-        <v>0.15315</v>
+        <v>0.21638</v>
       </c>
       <c r="C35" t="n">
-        <v>0.1629652096888499</v>
+        <v>0.2223350944354925</v>
       </c>
       <c r="D35" t="n">
-        <v>0.009815209688849885</v>
+        <v>0.005955094435492525</v>
       </c>
       <c r="E35" t="n">
-        <v>0.9902801922622315</v>
+        <v>0.9940801587780275</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B36" t="n">
-        <v>0.16299</v>
+        <v>0.17142</v>
       </c>
       <c r="C36" t="n">
-        <v>0.1734811551796907</v>
+        <v>0.1649602682526871</v>
       </c>
       <c r="D36" t="n">
-        <v>0.01049115517969071</v>
+        <v>0.00645973174731293</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9896177664436606</v>
+        <v>0.9935817285644422</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>0.23605</v>
+        <v>0.17029</v>
       </c>
       <c r="C37" t="n">
-        <v>0.2252660487682792</v>
+        <v>0.1636660381672836</v>
       </c>
       <c r="D37" t="n">
-        <v>0.01078395123172085</v>
+        <v>0.006623961832716407</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9893311016478054</v>
+        <v>0.9934196263114417</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B38" t="n">
-        <v>0.16861</v>
+        <v>0.17338</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1798844207808805</v>
+        <v>0.1665379255371373</v>
       </c>
       <c r="D38" t="n">
-        <v>0.01127442078088048</v>
+        <v>0.006842074462862752</v>
       </c>
       <c r="E38" t="n">
-        <v>0.9888512746399986</v>
+        <v>0.9932044213919915</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B39" t="n">
-        <v>0.19671</v>
+        <v>0.1672</v>
       </c>
       <c r="C39" t="n">
-        <v>0.2116945099043098</v>
+        <v>0.1742576594568286</v>
       </c>
       <c r="D39" t="n">
-        <v>0.01498450990430977</v>
+        <v>0.007057659456828597</v>
       </c>
       <c r="E39" t="n">
-        <v>0.9852367107496818</v>
+        <v>0.9929918020179349</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B40" t="n">
-        <v>0.21048</v>
+        <v>0.19109</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1952168851521131</v>
+        <v>0.1836756537298511</v>
       </c>
       <c r="D40" t="n">
-        <v>0.01526311484788692</v>
+        <v>0.007414346270148892</v>
       </c>
       <c r="E40" t="n">
-        <v>0.9849663455466184</v>
+        <v>0.9926402216748256</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B41" t="n">
-        <v>0.15315</v>
+        <v>0.20345</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1376430256785741</v>
+        <v>0.2110188873507921</v>
       </c>
       <c r="D41" t="n">
-        <v>0.01550697432142586</v>
+        <v>0.007568887350792058</v>
       </c>
       <c r="E41" t="n">
-        <v>0.9847298199682107</v>
+        <v>0.9924879703553641</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B42" t="n">
-        <v>0.21048</v>
+        <v>0.21244</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1931840507159756</v>
+        <v>0.2036841098322762</v>
       </c>
       <c r="D42" t="n">
-        <v>0.01729594928402442</v>
+        <v>0.00875589016772374</v>
       </c>
       <c r="E42" t="n">
-        <v>0.9829981144659061</v>
+        <v>0.9913201099958207</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B43" t="n">
-        <v>0.25853</v>
+        <v>0.18153</v>
       </c>
       <c r="C43" t="n">
-        <v>0.238700771253469</v>
+        <v>0.1698938860758195</v>
       </c>
       <c r="D43" t="n">
-        <v>0.01982922874653098</v>
+        <v>0.01163611392418051</v>
       </c>
       <c r="E43" t="n">
-        <v>0.9805563243456917</v>
+        <v>0.988497727825232</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B44" t="n">
-        <v>0.26134</v>
+        <v>0.18153</v>
       </c>
       <c r="C44" t="n">
-        <v>0.2407252874002477</v>
+        <v>0.1696123615841421</v>
       </c>
       <c r="D44" t="n">
-        <v>0.02061471259975234</v>
+        <v>0.01191763841585788</v>
       </c>
       <c r="E44" t="n">
-        <v>0.9798016701647955</v>
+        <v>0.9882227189610858</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B45" t="n">
-        <v>0.18266</v>
+        <v>0.22902</v>
       </c>
       <c r="C45" t="n">
-        <v>0.1595034233832925</v>
+        <v>0.2138717721090488</v>
       </c>
       <c r="D45" t="n">
-        <v>0.02315657661670753</v>
+        <v>0.01514822789095124</v>
       </c>
       <c r="E45" t="n">
-        <v>0.9773675142730551</v>
+        <v>0.9850778167416765</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B46" t="n">
-        <v>0.18266</v>
+        <v>0.15456</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1592282135463693</v>
+        <v>0.1356372788601496</v>
       </c>
       <c r="D46" t="n">
-        <v>0.02343178645363067</v>
+        <v>0.01892272113985036</v>
       </c>
       <c r="E46" t="n">
-        <v>0.9771046915253376</v>
+        <v>0.9814286984211307</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B47" t="n">
-        <v>0.26415</v>
+        <v>0.18856</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2308336948178446</v>
+        <v>0.1659385432086418</v>
       </c>
       <c r="D47" t="n">
-        <v>0.03331630518215542</v>
+        <v>0.02262145679135821</v>
       </c>
       <c r="E47" t="n">
-        <v>0.9677578830266476</v>
+        <v>0.9778789535060834</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B48" t="n">
-        <v>0.22762</v>
+        <v>0.18125</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1902944171052799</v>
+        <v>0.156975332970231</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0373255828947201</v>
+        <v>0.02427466702976899</v>
       </c>
       <c r="E48" t="n">
-        <v>0.9640174854354205</v>
+        <v>0.9763006273501214</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B49" t="n">
-        <v>0.31473</v>
+        <v>0.22368</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2008926003128128</v>
+        <v>0.1899030866869787</v>
       </c>
       <c r="D49" t="n">
-        <v>0.1138373996871872</v>
+        <v>0.0337769133130213</v>
       </c>
       <c r="E49" t="n">
-        <v>0.897797111392419</v>
+        <v>0.9673266902384443</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.11606</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.153914430608477</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.03785443060847701</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.963526261976563</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.1377</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.08446691207348882</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.05323308792651117</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.9494574481786262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>